<commit_message>
Resolução da Quarta Questão
</commit_message>
<xml_diff>
--- a/Dados/Questao2.xlsx
+++ b/Dados/Questao2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edevaldogaudencio/Documents/Pessoal/Educação/FGV/Mestrado Profissional em Economia/2_2020/Estatística/Listas de Exercícios/Lista 1/dados/MestradoEstatisticaLista1/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06163AFE-D47F-4F4A-92C5-9C5F2C39430E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468AA06A-4C01-784D-8AAC-8E97614208D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="460" windowWidth="27080" windowHeight="16040" xr2:uid="{6CD22184-46C3-6942-B6DE-114C9FA52279}"/>
   </bookViews>
@@ -514,7 +514,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>